<commit_message>
Fixed weird string encoding issue
</commit_message>
<xml_diff>
--- a/static/data.xlsx
+++ b/static/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sahithi/TrashArmy/flask-app/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sahithi/TrashArmy/TrashFrontEnd/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>col3</t>
+  </si>
+  <si>
+    <t>col4</t>
   </si>
 </sst>
 </file>
@@ -360,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +384,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20111001</v>
       </c>
@@ -395,8 +401,11 @@
       <c r="D2">
         <v>72.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>20111002</v>
       </c>
@@ -409,8 +418,11 @@
       <c r="D3">
         <v>67.599999999999994</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20111003</v>
       </c>
@@ -423,8 +435,11 @@
       <c r="D4">
         <v>69.400000000000006</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20111004</v>
       </c>
@@ -437,8 +452,11 @@
       <c r="D5">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20111005</v>
       </c>
@@ -451,8 +469,11 @@
       <c r="D6">
         <v>72.400000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20111006</v>
       </c>
@@ -465,8 +486,11 @@
       <c r="D7">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20111007</v>
       </c>
@@ -479,8 +503,11 @@
       <c r="D8">
         <v>82.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20111008</v>
       </c>
@@ -493,8 +520,11 @@
       <c r="D9">
         <v>78.900000000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20111009</v>
       </c>
@@ -507,8 +537,11 @@
       <c r="D10">
         <v>68.599999999999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20111010</v>
       </c>
@@ -521,8 +554,11 @@
       <c r="D11">
         <v>68.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20111011</v>
       </c>
@@ -535,8 +571,11 @@
       <c r="D12">
         <v>70.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20111012</v>
       </c>
@@ -549,8 +588,11 @@
       <c r="D13">
         <v>75.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20111013</v>
       </c>
@@ -563,8 +605,11 @@
       <c r="D14">
         <v>76.599999999999994</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20111014</v>
       </c>
@@ -577,8 +622,11 @@
       <c r="D15">
         <v>66.599999999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20111015</v>
       </c>
@@ -591,8 +639,11 @@
       <c r="D16">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20111016</v>
       </c>
@@ -605,8 +656,11 @@
       <c r="D17">
         <v>70.599999999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20111017</v>
       </c>
@@ -619,8 +673,11 @@
       <c r="D18">
         <v>71.099999999999994</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20111018</v>
       </c>
@@ -633,8 +690,11 @@
       <c r="D19">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20111019</v>
       </c>
@@ -647,8 +707,11 @@
       <c r="D20">
         <v>61.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20111020</v>
       </c>
@@ -661,8 +724,11 @@
       <c r="D21">
         <v>57.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20111021</v>
       </c>
@@ -675,8 +741,11 @@
       <c r="D22">
         <v>64.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20111022</v>
       </c>
@@ -688,6 +757,9 @@
       </c>
       <c r="D23">
         <v>72.400000000000006</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>